<commit_message>
summary.py: added charged/discharged kWh, using location to determine moved, small improvement in delta SOC
</commit_message>
<xml_diff>
--- a/examples/summary.day.xlsx
+++ b/examples/summary.day.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBDAA9E-B3D3-4C50-865A-AE4608147894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E09A6F3-11B0-4C89-9728-469FB4A72D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="summary.day" localSheetId="0">Sheet1!$A$1:$J$10</definedName>
+    <definedName name="summary.day" localSheetId="0">Sheet1!$A$1:$L$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -44,10 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
-  <si>
-    <t>Label</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t xml:space="preserve"> date      </t>
   </si>
@@ -61,12 +58,6 @@
     <t xml:space="preserve"> discharged%</t>
   </si>
   <si>
-    <t xml:space="preserve"> charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> drives</t>
-  </si>
-  <si>
     <t xml:space="preserve"> km/kWh</t>
   </si>
   <si>
@@ -74,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve"> cost Euro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAY  </t>
   </si>
   <si>
     <t xml:space="preserve"> 2022-09-17</t>
@@ -104,6 +92,24 @@
   </si>
   <si>
     <t xml:space="preserve"> 2022-09-25</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> charged kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> discharged kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #drives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAY   </t>
   </si>
 </sst>
 </file>
@@ -483,6 +489,330 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> cost Euro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v> 2022-09-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> 2022-09-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> 2022-09-19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> 2022-09-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> 2022-09-21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> 2022-09-22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> 2022-09-23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> 2022-09-24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> 2022-09-25</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B469-4193-860C-086383D461CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1654183695"/>
+        <c:axId val="1654184111"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1654183695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1654184111"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1654184111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1654183695"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -612,13 +942,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.37</c:v>
@@ -866,7 +1196,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> discharged%</c:v>
+                  <c:v> charged kWh</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -923,31 +1253,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>18.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>20.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-95</c:v>
+                  <c:v>25.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1190,7 +1520,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> charges</c:v>
+                  <c:v> discharged%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1244,31 +1574,31 @@
             <c:numRef>
               <c:f>Sheet1!$F$2:$F$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>-0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>-0.95</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1367,7 +1697,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1514,7 +1844,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> drives</c:v>
+                  <c:v> discharged kWh</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1577,22 +1907,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>-0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>-9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>-0.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>-0.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>-66.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1838,7 +2168,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> km/kWh</c:v>
+                  <c:v> #charges</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1895,7 +2225,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1904,19 +2234,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9000000000000004</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2162,7 +2492,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> kWh/100km</c:v>
+                  <c:v> #drives</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2225,22 +2555,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2486,7 +2816,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> cost Euro</c:v>
+                  <c:v> km/kWh</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2552,7 +2882,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.41</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2564,7 +2894,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.36</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2750,7 +3080,371 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> kWh/100km</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v> 2022-09-17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> 2022-09-18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> 2022-09-19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> 2022-09-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> 2022-09-21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> 2022-09-22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> 2022-09-23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> 2022-09-24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> 2022-09-25</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE37-4F52-957F-A808325CB7F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1561553231"/>
+        <c:axId val="1561558223"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1561553231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1561558223"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1561558223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1561553231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3070,6 +3764,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3586,8 +4320,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3695,11 +4429,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3710,11 +4439,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3746,9 +4470,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4102,8 +4823,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4211,6 +4932,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4221,6 +4947,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4252,6 +4983,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4605,7 +5339,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5108,7 +5842,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5611,7 +6345,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6114,7 +6848,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6617,7 +7351,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7120,17 +7854,1023 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>33337</xdr:rowOff>
@@ -7160,13 +8900,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
@@ -7196,13 +8936,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
@@ -7232,13 +8972,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
@@ -7268,16 +9008,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7304,16 +9044,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7340,16 +9080,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7376,16 +9116,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7405,6 +9145,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{514D3CDD-B02F-7EEA-3CEC-4E4017B2EF1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50803E62-E5B5-E517-7179-A9C5BC2F542E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7680,64 +9492,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -7746,16 +9566,16 @@
         <v>0.04</v>
       </c>
       <c r="E2">
+        <v>2.8</v>
+      </c>
+      <c r="F2" s="2">
         <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -7763,13 +9583,19 @@
       <c r="J2">
         <v>0</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -7778,9 +9604,9 @@
         <v>0.02</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+        <v>1.4</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3">
@@ -7795,13 +9621,19 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>6.5</v>
@@ -7812,28 +9644,34 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="F4" s="2">
+        <v>-0.01</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>-0.7</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5">
         <v>47.6</v>
@@ -7842,62 +9680,74 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>-14</v>
-      </c>
-      <c r="F5">
         <v>0</v>
       </c>
+      <c r="F5" s="2">
+        <v>-0.14000000000000001</v>
+      </c>
       <c r="G5">
+        <v>-9.8000000000000007</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>20.6</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>2.41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>5.2</v>
       </c>
       <c r="D6" s="2">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+        <v>18.2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="G6">
+        <v>-0.7</v>
+      </c>
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>2</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>1.9</v>
@@ -7906,62 +9756,74 @@
         <v>0.02</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+        <v>1.4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="G7">
+        <v>-0.7</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>1.7</v>
       </c>
       <c r="D8" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E8">
+        <v>20.3</v>
+      </c>
+      <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>407.8</v>
@@ -7970,30 +9832,36 @@
         <v>0.37</v>
       </c>
       <c r="E9">
-        <v>-95</v>
-      </c>
-      <c r="F9">
+        <v>25.9</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-0.95</v>
+      </c>
+      <c r="G9">
+        <v>-66.5</v>
+      </c>
+      <c r="H9">
         <v>1</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>6</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>6.1</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>16.3</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>16.36</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -8002,9 +9870,9 @@
         <v>0.08</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+        <v>5.6</v>
+      </c>
+      <c r="F10" s="2">
         <v>0</v>
       </c>
       <c r="G10">
@@ -8017,6 +9885,12 @@
         <v>0</v>
       </c>
       <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
summary.py: add averages for trip, day, week, month and prediction for year
</commit_message>
<xml_diff>
--- a/examples/summary.day.xlsx
+++ b/examples/summary.day.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7E1F67-2DCE-4520-909A-F92289FD1F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C53033C-695D-48DE-8FFC-69241443069B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,16 +65,7 @@
     <t xml:space="preserve"> cost Euro</t>
   </si>
   <si>
-    <t>Period</t>
-  </si>
-  <si>
     <t xml:space="preserve"> #charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> #drives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAY   </t>
   </si>
   <si>
     <t xml:space="preserve"> info </t>
@@ -140,7 +131,16 @@
     <t xml:space="preserve"> 12V%CUR</t>
   </si>
   <si>
-    <t xml:space="preserve"> #moves</t>
+    <t xml:space="preserve">  Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   #trips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   #moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAY     </t>
   </si>
 </sst>
 </file>
@@ -1276,13 +1276,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v> #moves</c:v>
+                  <c:v>   #moves</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>       </c:v>
+                  <c:v>         </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>       </c:v>
+                  <c:v>         </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2590,13 +2590,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v> #drives</c:v>
+                  <c:v>   #trips</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>        </c:v>
+                  <c:v>         </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>        </c:v>
+                  <c:v>         </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16874,12 +16874,12 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -16898,31 +16898,31 @@
     <col min="17" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.85546875" customWidth="1"/>
-    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -16934,69 +16934,69 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2">
         <v>44821</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3">
         <v>17324.2</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3">
         <v>2.8</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K2">
         <v>58</v>
@@ -17026,42 +17026,42 @@
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="U2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2">
         <v>44822</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3">
         <v>17324.2</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3">
         <v>0.7</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K3">
         <v>59</v>
@@ -17088,24 +17088,24 @@
         <v>91</v>
       </c>
       <c r="S3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="U3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2">
         <v>44823</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>17330.7</v>
@@ -17114,19 +17114,19 @@
         <v>6.5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K4">
         <v>59</v>
@@ -17153,7 +17153,7 @@
         <v>91</v>
       </c>
       <c r="S4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T4">
         <v>2</v>
@@ -17164,13 +17164,13 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2">
         <v>44824</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3">
         <v>17378.3</v>
@@ -17179,7 +17179,7 @@
         <v>47.6</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>-7</v>
@@ -17218,7 +17218,7 @@
         <v>92</v>
       </c>
       <c r="S5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T5">
         <v>3</v>
@@ -17229,13 +17229,13 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>44825</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3">
         <v>17383.5</v>
@@ -17250,13 +17250,13 @@
         <v>-0.7</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -17294,34 +17294,34 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>44826</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3">
         <v>17383.5</v>
       </c>
       <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K7">
         <v>72</v>
@@ -17351,21 +17351,21 @@
         <v>1</v>
       </c>
       <c r="T7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="U7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>44827</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3">
         <v>17387.099999999999</v>
@@ -17380,13 +17380,13 @@
         <v>-0.7</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K8">
         <v>100</v>
@@ -17424,13 +17424,13 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>44828</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3">
         <v>17794.900000000001</v>
@@ -17489,34 +17489,34 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>44829</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3">
         <v>17794.900000000001</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3">
         <v>5.6</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K10">
         <v>50</v>
@@ -17543,13 +17543,13 @@
         <v>97</v>
       </c>
       <c r="S10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="U10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major new release: Tripinfo from the car (Europe only) and other improvements
</commit_message>
<xml_diff>
--- a/examples/summary.day.xlsx
+++ b/examples/summary.day.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65E7CF0-C342-47BC-91FD-6585D33B6606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5529CBFF-F534-439C-9CF9-1AF27A3DD273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="summary.day_1" localSheetId="0">Sheet1!$A$1:$T$10</definedName>
+    <definedName name="summary.day_1" localSheetId="0">Sheet1!$A$1:$V$8</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
   <si>
     <t xml:space="preserve"> date      </t>
   </si>
@@ -101,22 +101,13 @@
     <t xml:space="preserve">        </t>
   </si>
   <si>
-    <t xml:space="preserve"> Thu  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Fri  </t>
   </si>
   <si>
     <t xml:space="preserve"> odometer</t>
   </si>
   <si>
-    <t xml:space="preserve"> SOC%CUR</t>
-  </si>
-  <si>
     <t>AVG</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12V%CUR</t>
   </si>
   <si>
     <t xml:space="preserve">  Period</t>
@@ -138,6 +129,24 @@
   </si>
   <si>
     <t xml:space="preserve"> Wed  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SOC%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12V%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EV range</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "9;Kwakstraat; Duckstad; Nederland; 7054; AN"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "7;Kwakstraat; Duckstad; Nederland; 7054; AN"</t>
   </si>
 </sst>
 </file>
@@ -273,73 +282,117 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$10</c:f>
+              <c:f>Sheet1!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5</c:v>
+                  <c:v>155.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.6</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10.199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>407.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -363,14 +416,14 @@
         <c:axId val="2124121984"/>
         <c:axId val="2124124896"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2124121984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -410,9 +463,10 @@
         <c:crossAx val="2124124896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2124124896"/>
         <c:scaling>
@@ -621,74 +675,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$10</c:f>
+              <c:f>Sheet1!$M$2:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -712,14 +810,14 @@
         <c:axId val="1654183695"/>
         <c:axId val="1654184111"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="1654183695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -759,9 +857,10 @@
         <c:crossAx val="1654184111"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1654184111"/>
         <c:scaling>
@@ -970,74 +1069,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$2:$R$10</c:f>
+              <c:f>Sheet1!$R$2:$R$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>97</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,14 +1204,14 @@
         <c:axId val="994887136"/>
         <c:axId val="994902528"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="994887136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1108,9 +1251,10 @@
         <c:crossAx val="994902528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="994902528"/>
         <c:scaling>
@@ -1319,74 +1463,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$10</c:f>
+              <c:f>Sheet1!$N$2:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>61</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1410,14 +1598,14 @@
         <c:axId val="1654183695"/>
         <c:axId val="1654184111"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="1654183695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1457,9 +1645,10 @@
         <c:crossAx val="1654184111"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1654184111"/>
         <c:scaling>
@@ -1644,73 +1833,60 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>17324.2</c:v>
+                  <c:v>22163.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17324.2</c:v>
+                  <c:v>22167.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17330.7</c:v>
+                  <c:v>22323</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17378.3</c:v>
+                  <c:v>22328.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17383.5</c:v>
+                  <c:v>22334.400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17383.5</c:v>
+                  <c:v>22344.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17387.099999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17794.900000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17794.900000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,14 +1909,14 @@
         <c:axId val="2124121984"/>
         <c:axId val="2124124896"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2124121984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1780,9 +1956,10 @@
         <c:crossAx val="2124124896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2124124896"/>
         <c:scaling>
@@ -1951,7 +2128,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 12V%CUR</c:v>
+                  <c:v> 12V%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1966,74 +2143,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$10</c:f>
+              <c:f>Sheet1!$O$2:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>91</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>91</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>97</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2057,14 +2278,14 @@
         <c:axId val="2129261072"/>
         <c:axId val="2129253584"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2129261072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2104,9 +2325,10 @@
         <c:crossAx val="2129253584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2129253584"/>
         <c:scaling>
@@ -2290,73 +2512,117 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$10</c:f>
+              <c:f>Sheet1!$T$2:$T$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2381,14 +2647,14 @@
         <c:axId val="740828864"/>
         <c:axId val="740831776"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="740828864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2428,9 +2694,10 @@
         <c:crossAx val="740831776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="740831776"/>
         <c:scaling>
@@ -2614,73 +2881,117 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$2:$S$10</c:f>
+              <c:f>Sheet1!$S$2:$S$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2705,14 +3016,14 @@
         <c:axId val="740828864"/>
         <c:axId val="740831776"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="740828864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2752,9 +3063,10 @@
         <c:crossAx val="740831776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="740831776"/>
         <c:scaling>
@@ -2938,48 +3250,98 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$10</c:f>
+              <c:f>Sheet1!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2987,10 +3349,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2999,12 +3361,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3029,14 +3385,14 @@
         <c:axId val="2129256080"/>
         <c:axId val="2129257744"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2129256080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3076,9 +3432,10 @@
         <c:crossAx val="2129257744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2129257744"/>
         <c:scaling>
@@ -3262,74 +3619,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$10</c:f>
+              <c:f>Sheet1!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3352,14 +3753,14 @@
         <c:axId val="2129256496"/>
         <c:axId val="2129251504"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2129256496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3399,9 +3800,10 @@
         <c:crossAx val="2129251504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2129251504"/>
         <c:scaling>
@@ -3585,73 +3987,117 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$10</c:f>
+              <c:f>Sheet1!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-0.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-26.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7</c:v>
+                  <c:v>-1.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.7</c:v>
+                  <c:v>-1.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-1.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-66.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3676,14 +4122,14 @@
         <c:axId val="2137395376"/>
         <c:axId val="2137388304"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2137395376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3723,9 +4169,10 @@
         <c:crossAx val="2137388304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2137388304"/>
         <c:scaling>
@@ -3934,74 +4381,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$10</c:f>
+              <c:f>Sheet1!$P$2:$P$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>88</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>91</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>97</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4025,14 +4516,14 @@
         <c:axId val="2129261072"/>
         <c:axId val="2129253584"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2129261072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4072,9 +4563,10 @@
         <c:crossAx val="2129253584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2129253584"/>
         <c:scaling>
@@ -4283,74 +4775,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$10</c:f>
+              <c:f>Sheet1!$Q$2:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>97</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4374,14 +4910,14 @@
         <c:axId val="2137408688"/>
         <c:axId val="2137401616"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2137408688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4421,9 +4957,10 @@
         <c:crossAx val="2137401616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2137401616"/>
         <c:scaling>
@@ -4607,48 +5144,98 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$10</c:f>
+              <c:f>Sheet1!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4656,10 +5243,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4668,12 +5255,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4698,14 +5279,14 @@
         <c:axId val="2129256080"/>
         <c:axId val="2129257744"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2129256080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4745,9 +5326,10 @@
         <c:crossAx val="2129257744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2129257744"/>
         <c:scaling>
@@ -4931,48 +5513,98 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$10</c:f>
+              <c:f>Sheet1!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4980,10 +5612,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.72</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4992,12 +5624,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16.36</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5022,14 +5648,14 @@
         <c:axId val="2131867888"/>
         <c:axId val="2131865392"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2131867888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5069,9 +5695,10 @@
         <c:crossAx val="2131865392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2131865392"/>
         <c:scaling>
@@ -5240,7 +5867,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> SOC%CUR</c:v>
+                  <c:v> SOC%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5255,74 +5882,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$10</c:f>
+              <c:f>Sheet1!$K$2:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5346,14 +6017,14 @@
         <c:axId val="100937328"/>
         <c:axId val="100951472"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="100937328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5393,9 +6064,10 @@
         <c:crossAx val="100951472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="100951472"/>
         <c:scaling>
@@ -5604,74 +6276,118 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>44821</c:v>
+                  <c:v>13-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44822</c:v>
+                  <c:v>14-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44823</c:v>
+                  <c:v>15-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44824</c:v>
+                  <c:v>16-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44825</c:v>
+                  <c:v>17-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44826</c:v>
+                  <c:v>18-1-2023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44827</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44829</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v> date      </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$10</c:f>
+              <c:f>Sheet1!$L$2:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>72</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>50</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5695,14 +6411,14 @@
         <c:axId val="1561553231"/>
         <c:axId val="1561558223"/>
       </c:barChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="1561553231"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5742,9 +6458,10 @@
         <c:crossAx val="1561558223"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1561558223"/>
         <c:scaling>
@@ -15127,16 +15844,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15163,16 +15880,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15199,16 +15916,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15235,16 +15952,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>396816</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>147097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15271,16 +15988,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>63081</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>156623</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>209011</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15307,16 +16024,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>2809876</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15343,16 +16060,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15379,16 +16096,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>401668</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15415,16 +16132,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>396277</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>168304</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15451,16 +16168,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>60385</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>176752</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15487,16 +16204,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>222729</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>155524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15523,16 +16240,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>241181</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15562,15 +16279,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
+      <xdr:colOff>142874</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15600,14 +16317,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>383157</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15637,16 +16354,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15676,14 +16393,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15713,16 +16430,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200026</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16019,10 +16736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD47" sqref="AD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16037,22 +16754,23 @@
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -16061,7 +16779,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -16082,10 +16800,10 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
         <v>9</v>
@@ -16094,10 +16812,10 @@
         <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q1" t="s">
         <v>9</v>
@@ -16109,27 +16827,33 @@
         <v>4</v>
       </c>
       <c r="T1" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2">
-        <v>44821</v>
+        <v>44939</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3">
-        <v>17324.2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3">
-        <v>2.8</v>
+        <v>22163.4</v>
+      </c>
+      <c r="E2">
+        <v>1.2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -16147,54 +16871,60 @@
         <v>58</v>
       </c>
       <c r="L2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M2">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N2">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O2">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P2">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q2">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="R2">
-        <v>91</v>
-      </c>
-      <c r="S2">
+        <v>89</v>
+      </c>
+      <c r="S2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2">
         <v>1</v>
       </c>
-      <c r="T2" t="s">
-        <v>12</v>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2">
+        <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2">
-        <v>44822</v>
+        <v>44940</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3">
-        <v>17324.2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
+        <v>22167.5</v>
+      </c>
+      <c r="E3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>-0.7</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -16206,181 +16936,199 @@
         <v>14</v>
       </c>
       <c r="K3">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L3">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M3">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N3">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O3">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P3">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q3">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R3">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S3" t="s">
         <v>12</v>
       </c>
-      <c r="T3" t="s">
-        <v>12</v>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3">
+        <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
-        <v>44823</v>
+        <v>44941</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3">
-        <v>17330.7</v>
+        <v>22323</v>
       </c>
       <c r="E4">
-        <v>6.5</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
+        <v>155.5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>33.6</v>
+      </c>
+      <c r="G4">
+        <v>-26.6</v>
+      </c>
+      <c r="H4">
+        <v>5.8</v>
+      </c>
+      <c r="I4">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="J4">
+        <v>6.54</v>
       </c>
       <c r="K4">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="L4">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="M4">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="N4">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="O4">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="P4">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="Q4">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="R4">
-        <v>91</v>
-      </c>
-      <c r="S4" t="s">
-        <v>12</v>
+        <v>95</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="U4" t="s">
+        <v>30</v>
+      </c>
+      <c r="V4">
+        <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2">
-        <v>44824</v>
+        <v>44942</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3">
-        <v>17378.3</v>
+        <v>22328.6</v>
       </c>
       <c r="E5">
-        <v>47.6</v>
+        <v>5.6</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G5">
-        <v>-7</v>
-      </c>
-      <c r="H5">
-        <v>6.8</v>
-      </c>
-      <c r="I5">
-        <v>14.7</v>
-      </c>
-      <c r="J5">
-        <v>1.72</v>
+        <v>-1.4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
       </c>
       <c r="K5">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="L5">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="M5">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="N5">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="O5">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="P5">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q5">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="R5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="S5" t="s">
         <v>12</v>
       </c>
       <c r="T5">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="U5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5">
+        <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44943</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2">
-        <v>44825</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="3">
-        <v>17383.5</v>
+        <v>22334.400000000001</v>
       </c>
       <c r="E6">
-        <v>5.2</v>
-      </c>
-      <c r="F6" s="3">
-        <v>18.2</v>
+        <v>5.8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="G6">
-        <v>-0.7</v>
+        <v>-1.4</v>
       </c>
       <c r="H6" t="s">
         <v>13</v>
@@ -16392,57 +17140,63 @@
         <v>14</v>
       </c>
       <c r="K6">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="L6">
+        <v>64</v>
+      </c>
+      <c r="M6">
         <v>63</v>
       </c>
-      <c r="M6">
-        <v>46</v>
-      </c>
       <c r="N6">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O6">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P6">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="Q6">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="R6">
-        <v>92</v>
-      </c>
-      <c r="S6">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="S6" t="s">
+        <v>12</v>
       </c>
       <c r="T6">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>30</v>
+      </c>
+      <c r="V6">
+        <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>44826</v>
+        <v>44944</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3">
-        <v>17383.5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
+        <v>22344.6</v>
+      </c>
+      <c r="E7">
+        <v>10.199999999999999</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
-        <v>12</v>
+      <c r="G7">
+        <v>-1.4</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -16454,220 +17208,108 @@
         <v>14</v>
       </c>
       <c r="K7">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="L7">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="M7">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="N7">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="O7">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="P7">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q7">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="R7">
-        <v>91</v>
-      </c>
-      <c r="S7">
+        <v>89</v>
+      </c>
+      <c r="S7" t="s">
+        <v>12</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7" t="s">
+        <v>30</v>
+      </c>
+      <c r="V7">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
         <v>1</v>
       </c>
-      <c r="T7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2">
-        <v>44827</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3">
-        <v>17387.099999999999</v>
-      </c>
-      <c r="E8">
-        <v>3.6</v>
-      </c>
-      <c r="F8" s="3">
-        <v>20.3</v>
-      </c>
-      <c r="G8">
-        <v>-0.7</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8">
-        <v>100</v>
-      </c>
-      <c r="L8">
-        <v>86</v>
-      </c>
-      <c r="M8">
-        <v>71</v>
-      </c>
-      <c r="N8">
-        <v>100</v>
-      </c>
-      <c r="O8">
-        <v>87</v>
-      </c>
-      <c r="P8">
-        <v>87</v>
-      </c>
-      <c r="Q8">
-        <v>87</v>
-      </c>
-      <c r="R8">
-        <v>88</v>
-      </c>
-      <c r="S8">
-        <v>2</v>
-      </c>
-      <c r="T8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
-        <v>44828</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3">
-        <v>17794.900000000001</v>
-      </c>
-      <c r="E9">
-        <v>407.8</v>
-      </c>
-      <c r="F9" s="3">
-        <v>25.9</v>
-      </c>
-      <c r="G9">
-        <v>-66.5</v>
-      </c>
-      <c r="H9">
-        <v>6.1</v>
-      </c>
-      <c r="I9">
-        <v>16.3</v>
-      </c>
-      <c r="J9">
-        <v>16.36</v>
-      </c>
-      <c r="K9">
-        <v>42</v>
-      </c>
-      <c r="L9">
-        <v>40</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
-      <c r="N9">
-        <v>100</v>
-      </c>
-      <c r="O9">
-        <v>97</v>
-      </c>
-      <c r="P9">
-        <v>96</v>
-      </c>
-      <c r="Q9">
-        <v>92</v>
-      </c>
-      <c r="R9">
-        <v>98</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2">
-        <v>44829</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3">
-        <v>17794.900000000001</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="3">
-        <v>5.6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10">
-        <v>50</v>
-      </c>
-      <c r="L10">
-        <v>50</v>
-      </c>
-      <c r="M10">
-        <v>43</v>
-      </c>
-      <c r="N10">
-        <v>50</v>
-      </c>
-      <c r="O10">
-        <v>97</v>
-      </c>
-      <c r="P10">
-        <v>97</v>
-      </c>
-      <c r="Q10">
-        <v>97</v>
-      </c>
-      <c r="R10">
-        <v>97</v>
-      </c>
-      <c r="S10" t="s">
-        <v>12</v>
-      </c>
-      <c r="T10" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>